<commit_message>
Fixing unit tests except processor test
</commit_message>
<xml_diff>
--- a/Tests/Fixtures/01_fixture.xlsx
+++ b/Tests/Fixtures/01_fixture.xlsx
@@ -1,24 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thorsten\Documents\Projekte\typo3-extensions\spreadsheets\Tests\Fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D457BC-5752-4B42-B90A-FC164654EBF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixture1" sheetId="2" r:id="rId1"/>
     <sheet name="Fixture2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -121,7 +128,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="#,##0.0\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
@@ -129,7 +136,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.0\ [$₽-419]"/>
     <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="169" formatCode="0.0E+00"/>
-    <numFmt numFmtId="171" formatCode="0.000E+00"/>
+    <numFmt numFmtId="170" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -355,6 +362,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -367,7 +375,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -651,11 +658,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,10 +697,10 @@
       <c r="C2" s="3">
         <v>70</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="27">
         <v>80</v>
       </c>
-      <c r="E2" s="26"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
@@ -718,11 +725,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>5</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>7</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
@@ -732,7 +739,7 @@
       <c r="A6" s="7">
         <v>2014</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="28">
         <v>2015</v>
       </c>
       <c r="C6" s="8">
@@ -752,7 +759,7 @@
       <c r="A7" s="10">
         <v>50</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="11">
         <v>70</v>
       </c>
@@ -772,7 +779,7 @@
     <mergeCell ref="B6:B7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -780,7 +787,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -798,10 +805,10 @@
       <c r="B1">
         <v>456</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -894,7 +901,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="30">
+      <c r="C9" s="26">
         <f>B2</f>
         <v>579</v>
       </c>

</xml_diff>

<commit_message>
Improve test coverage and logic for existing test cases
</commit_message>
<xml_diff>
--- a/Tests/Fixtures/01_fixture.xlsx
+++ b/Tests/Fixtures/01_fixture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thorsten\Documents\Projekte\typo3-extensions\spreadsheets\Tests\Fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\thorsten\projects\typo3\spreadsheets\Tests\Fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D457BC-5752-4B42-B90A-FC164654EBF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E02DC3-DE86-494A-AA6E-7E7E32BE21AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6132" yWindow="2760" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixture1" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>x</t>
   </si>
@@ -124,6 +127,12 @@
   <si>
     <t>Wissenschaftlich #2</t>
   </si>
+  <si>
+    <t>striked</t>
+  </si>
+  <si>
+    <t>centerized</t>
+  </si>
 </sst>
 </file>
 
@@ -138,7 +147,7 @@
     <numFmt numFmtId="169" formatCode="0.0E+00"/>
     <numFmt numFmtId="170" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +232,14 @@
     <font>
       <vertAlign val="subscript"/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -329,7 +346,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -374,6 +391,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -659,18 +680,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="11.42578125" style="5"/>
+    <col min="6" max="6" width="11.44140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>2014</v>
       </c>
@@ -687,7 +708,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>50</v>
       </c>
@@ -705,12 +726,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="G3" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
@@ -724,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D5" s="18" t="s">
         <v>7</v>
       </c>
@@ -735,7 +756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>2014</v>
       </c>
@@ -754,8 +775,11 @@
       <c r="F6" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>50</v>
       </c>
@@ -773,10 +797,31 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A9:G10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -792,13 +837,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>123</v>
       </c>
@@ -810,7 +855,7 @@
       </c>
       <c r="D1" s="30"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -826,7 +871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -842,7 +887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -858,7 +903,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -874,7 +919,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C6" s="22">
         <f>B5</f>
         <v>3.7073170731707319</v>
@@ -883,7 +928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7" s="23">
         <f>B5</f>
         <v>3.7073170731707319</v>
@@ -892,7 +937,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8" s="24">
         <v>43544</v>
       </c>
@@ -900,7 +945,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9" s="26">
         <f>B2</f>
         <v>579</v>

</xml_diff>

<commit_message>
Add unit tests for viewhelpers
</commit_message>
<xml_diff>
--- a/Tests/Fixtures/01_fixture.xlsx
+++ b/Tests/Fixtures/01_fixture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\thorsten\projects\typo3\spreadsheets\Tests\Fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Devbox\home\thorsten\projects\typo3\spreadsheets\Tests\Fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E02DC3-DE86-494A-AA6E-7E7E32BE21AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3D04C5-03C4-4CA7-939E-23C61DB06A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6132" yWindow="2760" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixture1" sheetId="2" r:id="rId1"/>
@@ -147,7 +147,7 @@
     <numFmt numFmtId="169" formatCode="0.0E+00"/>
     <numFmt numFmtId="170" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +240,14 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -360,9 +368,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -380,6 +385,7 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -390,11 +396,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -683,7 +691,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,13 +740,13 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -746,17 +754,17 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>5</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>2014</v>
       </c>
@@ -769,28 +777,28 @@
       <c r="D6" s="8">
         <v>2017</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="32">
         <v>2018</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="26" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>50</v>
       </c>
       <c r="B7" s="29"/>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>70</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>80</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>90</v>
       </c>
       <c r="G7" t="s">
@@ -798,24 +806,24 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -850,10 +858,10 @@
       <c r="B1">
         <v>456</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="30"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -863,7 +871,7 @@
         <f>A1+B1</f>
         <v>579</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="24">
         <f>B2</f>
         <v>579</v>
       </c>
@@ -879,7 +887,7 @@
         <f>A1-B1</f>
         <v>-333</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="18">
         <f>B3</f>
         <v>-333</v>
       </c>
@@ -895,7 +903,7 @@
         <f>A1*B1</f>
         <v>56088</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <f>B4</f>
         <v>56088</v>
       </c>
@@ -911,7 +919,7 @@
         <f>B1/A1</f>
         <v>3.7073170731707319</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <f>B5</f>
         <v>3.7073170731707319</v>
       </c>
@@ -920,7 +928,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <f>B5</f>
         <v>3.7073170731707319</v>
       </c>
@@ -929,7 +937,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C7" s="23">
+      <c r="C7" s="22">
         <f>B5</f>
         <v>3.7073170731707319</v>
       </c>
@@ -938,7 +946,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <v>43544</v>
       </c>
       <c r="D8" t="s">
@@ -946,7 +954,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" s="26">
+      <c r="C9" s="25">
         <f>B2</f>
         <v>579</v>
       </c>

</xml_diff>

<commit_message>
Fix rowspan/colspan breaking html table view
</commit_message>
<xml_diff>
--- a/Tests/Fixtures/01_fixture.xlsx
+++ b/Tests/Fixtures/01_fixture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Devbox\home\thorsten\projects\typo3\spreadsheets\Tests\Fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3D04C5-03C4-4CA7-939E-23C61DB06A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAA3990-C309-433B-A2DE-33888D25B87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>x</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>centerized</t>
+  </si>
+  <si>
+    <t>test after double rowspan</t>
   </si>
 </sst>
 </file>
@@ -386,6 +389,9 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,9 +406,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -688,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -726,10 +729,10 @@
       <c r="C2" s="3">
         <v>70</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="28">
         <v>80</v>
       </c>
-      <c r="E2" s="27"/>
+      <c r="E2" s="28"/>
       <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
@@ -768,7 +771,7 @@
       <c r="A6" s="7">
         <v>2014</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="29">
         <v>2015</v>
       </c>
       <c r="C6" s="8">
@@ -777,7 +780,7 @@
       <c r="D6" s="8">
         <v>2017</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="27">
         <v>2018</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -791,7 +794,7 @@
       <c r="A7" s="9">
         <v>50</v>
       </c>
-      <c r="B7" s="29"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="10">
         <v>70</v>
       </c>
@@ -806,24 +809,29 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -858,10 +866,10 @@
       <c r="B1">
         <v>456</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>